<commit_message>
commit progress update #761
</commit_message>
<xml_diff>
--- a/src/test/resources/metadata.xlsx
+++ b/src/test/resources/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sal153/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sal153/IdeaProjects/ecodata/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132FE184-3720-E849-8331-FB71748662FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{313C58CC-7876-BA49-871E-C3ED5616C5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{7B014210-C77D-C644-9901-B304ADE2D0C4}"/>
+    <workbookView xWindow="6180" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{7B014210-C77D-C644-9901-B304ADE2D0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,47 +35,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>joseph salomon</t>
-  </si>
-  <si>
-    <t>roma salomon</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>startDate</t>
-  </si>
-  <si>
-    <t>endDate</t>
-  </si>
-  <si>
-    <t>grantId</t>
-  </si>
-  <si>
-    <t>test1 desc</t>
-  </si>
-  <si>
-    <t>test2 desc</t>
-  </si>
-  <si>
-    <t>DD-01-D1</t>
-  </si>
-  <si>
-    <t>DD-02-D2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+  <si>
+    <t>management_unit</t>
+  </si>
+  <si>
+    <t>As is</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Project Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This column describes the name of the management unit used for the geographic region (NLP 2018), or the organisation unit responsible for activities in the area (but can reach into other geographic regions)  </t>
+  </si>
+  <si>
+    <t>Condamine</t>
+  </si>
+  <si>
+    <t>grant_id</t>
+  </si>
+  <si>
+    <t>This column describes the human readable unique ID assigned to a project</t>
+  </si>
+  <si>
+    <t>RLP-MU46-P2</t>
+  </si>
+  <si>
+    <t>activity_id</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>This column describes the program under which the project is being conducted (i.e. source of funding)</t>
+  </si>
+  <si>
+    <t>National Landcare Program</t>
+  </si>
+  <si>
+    <t>sub_program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This column describes the sub-program under which the project is being conducted </t>
+  </si>
+  <si>
+    <t>Regional Land Partnerships</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Column</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -105,7 +155,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,67 +470,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A0641B-7541-7C45-BF2A-7918413D7453}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44739</v>
-      </c>
-      <c r="D2" s="1">
-        <v>45107</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44739</v>
-      </c>
-      <c r="D3" s="1">
-        <v>45107</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>